<commit_message>
so much has changed
</commit_message>
<xml_diff>
--- a/bad_dk.xlsx
+++ b/bad_dk.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/p4lawren/Desktop/coding/research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EECCE7-4B77-F447-A9C0-8B14CFDDA047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213F2C9A-D78A-A440-B300-217649D62C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="780" windowWidth="38400" windowHeight="19460" activeTab="1" xr2:uid="{57C0059A-3D3E-2440-9BA3-03937EADE4BD}"/>
+    <workbookView xWindow="520" yWindow="1000" windowWidth="38400" windowHeight="19460" activeTab="2" xr2:uid="{57C0059A-3D3E-2440-9BA3-03937EADE4BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>R_i1</t>
   </si>
@@ -98,7 +100,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -386,7 +388,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -396,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4EF90D2-7953-E441-8DE6-95A1B1C33C10}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C15" sqref="A1:C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,10 +563,10 @@
         <v>10</v>
       </c>
       <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="C15">
         <v>200</v>
-      </c>
-      <c r="C15">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -576,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7077B70F-A5FE-9249-AC00-21DBB4C2EA28}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,13 +597,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -609,10 +611,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -620,21 +622,91 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A7F327-2B15-3E4B-A198-223F34DD640E}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
         <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>